<commit_message>
NYTC dataset related changes.
</commit_message>
<xml_diff>
--- a/sql/picube_trip/Pyramid-psql/zoo.xlsx
+++ b/sql/picube_trip/Pyramid-psql/zoo.xlsx
@@ -939,12 +939,12 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16" width="3.7109375" style="1" customWidth="1"/>
+    <col min="1" max="16" width="3.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="20.100000000000001" customHeight="1">

</xml_diff>